<commit_message>
Continued to do EDA and did linear regression
</commit_message>
<xml_diff>
--- a/DataSheet.xlsx
+++ b/DataSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marco\Documents\Code\HousePrices\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB22DDD3-EF23-46DD-A053-B2D6D928625A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{942855A5-5AD9-494B-8CA0-8DC77143279B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16455" yWindow="5985" windowWidth="21600" windowHeight="11400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="4200" windowWidth="21600" windowHeight="11400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="104">
   <si>
     <t>Description</t>
   </si>
@@ -283,6 +283,60 @@
   </si>
   <si>
     <t>PavedDrive</t>
+  </si>
+  <si>
+    <t>WoodDeckSF</t>
+  </si>
+  <si>
+    <t>OpenPorchSF</t>
+  </si>
+  <si>
+    <t>EnclosedPorch</t>
+  </si>
+  <si>
+    <t>3SsnPorch</t>
+  </si>
+  <si>
+    <t>ScreenPorch</t>
+  </si>
+  <si>
+    <t>PoolArea</t>
+  </si>
+  <si>
+    <t>PoolQC</t>
+  </si>
+  <si>
+    <t>Fence</t>
+  </si>
+  <si>
+    <t>MiscFeature</t>
+  </si>
+  <si>
+    <t>MiscVal</t>
+  </si>
+  <si>
+    <t>NoSold</t>
+  </si>
+  <si>
+    <t>YrSold</t>
+  </si>
+  <si>
+    <t>SaleType</t>
+  </si>
+  <si>
+    <t>SaleCondition</t>
+  </si>
+  <si>
+    <t>Little</t>
+  </si>
+  <si>
+    <t>medium</t>
+  </si>
+  <si>
+    <t>HIgh</t>
+  </si>
+  <si>
+    <t>GrLivArea</t>
   </si>
 </sst>
 </file>
@@ -616,10 +670,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:I67"/>
+  <dimension ref="B3:I82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68"/>
+    <sheetView tabSelected="1" topLeftCell="D7" workbookViewId="0">
+      <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -721,6 +775,9 @@
       <c r="F7" t="s">
         <v>21</v>
       </c>
+      <c r="G7" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
@@ -831,6 +888,9 @@
       <c r="F14" t="s">
         <v>21</v>
       </c>
+      <c r="G14" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
@@ -860,7 +920,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>35</v>
       </c>
@@ -874,7 +934,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>36</v>
       </c>
@@ -888,7 +948,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>37</v>
       </c>
@@ -901,8 +961,11 @@
       <c r="F19" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>38</v>
       </c>
@@ -915,8 +978,11 @@
       <c r="F20" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G20" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>39</v>
       </c>
@@ -929,8 +995,11 @@
       <c r="F21" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>40</v>
       </c>
@@ -944,7 +1013,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>41</v>
       </c>
@@ -958,7 +1027,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>42</v>
       </c>
@@ -972,7 +1041,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>43</v>
       </c>
@@ -986,7 +1055,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>44</v>
       </c>
@@ -1000,7 +1069,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>45</v>
       </c>
@@ -1014,7 +1083,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>46</v>
       </c>
@@ -1028,7 +1097,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>47</v>
       </c>
@@ -1042,7 +1111,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>48</v>
       </c>
@@ -1056,7 +1125,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>49</v>
       </c>
@@ -1070,7 +1139,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>50</v>
       </c>
@@ -1084,7 +1153,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>51</v>
       </c>
@@ -1098,7 +1167,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>52</v>
       </c>
@@ -1112,7 +1181,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>53</v>
       </c>
@@ -1126,7 +1195,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>54</v>
       </c>
@@ -1140,7 +1209,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>55</v>
       </c>
@@ -1154,7 +1223,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>56</v>
       </c>
@@ -1168,7 +1237,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>57</v>
       </c>
@@ -1182,7 +1251,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>58</v>
       </c>
@@ -1195,8 +1264,11 @@
       <c r="F40" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G40" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>59</v>
       </c>
@@ -1210,7 +1282,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>60</v>
       </c>
@@ -1224,7 +1296,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>61</v>
       </c>
@@ -1238,7 +1310,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>62</v>
       </c>
@@ -1252,7 +1324,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>63</v>
       </c>
@@ -1266,7 +1338,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>64</v>
       </c>
@@ -1280,7 +1352,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>65</v>
       </c>
@@ -1294,283 +1366,511 @@
         <v>15</v>
       </c>
     </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
+        <v>103</v>
+      </c>
+      <c r="D48" t="s">
+        <v>18</v>
+      </c>
+      <c r="E48" t="s">
+        <v>10</v>
+      </c>
+      <c r="F48" t="s">
+        <v>102</v>
+      </c>
+      <c r="G48" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
         <v>66</v>
       </c>
-      <c r="D48" t="s">
-        <v>18</v>
-      </c>
-      <c r="E48" t="s">
-        <v>10</v>
-      </c>
-      <c r="F48" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
+      <c r="D49" t="s">
+        <v>18</v>
+      </c>
+      <c r="E49" t="s">
+        <v>10</v>
+      </c>
+      <c r="F49" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
         <v>67</v>
       </c>
-      <c r="D49" t="s">
-        <v>18</v>
-      </c>
-      <c r="E49" t="s">
-        <v>10</v>
-      </c>
-      <c r="F49" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
+      <c r="D50" t="s">
+        <v>18</v>
+      </c>
+      <c r="E50" t="s">
+        <v>10</v>
+      </c>
+      <c r="F50" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
         <v>68</v>
       </c>
-      <c r="D50" t="s">
-        <v>18</v>
-      </c>
-      <c r="E50" t="s">
-        <v>10</v>
-      </c>
-      <c r="F50" t="s">
+      <c r="D51" t="s">
+        <v>18</v>
+      </c>
+      <c r="E51" t="s">
+        <v>10</v>
+      </c>
+      <c r="F51" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
+      <c r="G51" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
         <v>69</v>
       </c>
-      <c r="D51" t="s">
-        <v>18</v>
-      </c>
-      <c r="E51" t="s">
-        <v>10</v>
-      </c>
-      <c r="F51" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
+      <c r="D52" t="s">
+        <v>18</v>
+      </c>
+      <c r="E52" t="s">
+        <v>10</v>
+      </c>
+      <c r="F52" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
         <v>70</v>
       </c>
-      <c r="D52" t="s">
-        <v>18</v>
-      </c>
-      <c r="E52" t="s">
-        <v>10</v>
-      </c>
-      <c r="F52" t="s">
+      <c r="D53" t="s">
+        <v>18</v>
+      </c>
+      <c r="E53" t="s">
+        <v>10</v>
+      </c>
+      <c r="F53" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
+      <c r="G53" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
         <v>71</v>
       </c>
-      <c r="D53" t="s">
-        <v>18</v>
-      </c>
-      <c r="E53" t="s">
-        <v>10</v>
-      </c>
-      <c r="F53" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
+      <c r="D54" t="s">
+        <v>18</v>
+      </c>
+      <c r="E54" t="s">
+        <v>10</v>
+      </c>
+      <c r="F54" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
         <v>72</v>
       </c>
-      <c r="D54" t="s">
-        <v>9</v>
-      </c>
-      <c r="E54" t="s">
-        <v>10</v>
-      </c>
-      <c r="F54" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
+      <c r="D55" t="s">
+        <v>9</v>
+      </c>
+      <c r="E55" t="s">
+        <v>10</v>
+      </c>
+      <c r="F55" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
         <v>73</v>
       </c>
-      <c r="D55" t="s">
-        <v>18</v>
-      </c>
-      <c r="E55" t="s">
-        <v>10</v>
-      </c>
-      <c r="F55" t="s">
+      <c r="D56" t="s">
+        <v>18</v>
+      </c>
+      <c r="E56" t="s">
+        <v>10</v>
+      </c>
+      <c r="F56" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B56" t="s">
+      <c r="G56" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
         <v>74</v>
       </c>
-      <c r="D56" t="s">
-        <v>9</v>
-      </c>
-      <c r="E56" t="s">
-        <v>10</v>
-      </c>
-      <c r="F56" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B57" t="s">
+      <c r="D57" t="s">
+        <v>9</v>
+      </c>
+      <c r="E57" t="s">
+        <v>10</v>
+      </c>
+      <c r="F57" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
         <v>75</v>
       </c>
-      <c r="D57" t="s">
-        <v>18</v>
-      </c>
-      <c r="E57" t="s">
-        <v>10</v>
-      </c>
-      <c r="F57" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B58" t="s">
+      <c r="D58" t="s">
+        <v>18</v>
+      </c>
+      <c r="E58" t="s">
+        <v>10</v>
+      </c>
+      <c r="F58" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
         <v>76</v>
       </c>
-      <c r="D58" t="s">
-        <v>9</v>
-      </c>
-      <c r="E58" t="s">
-        <v>10</v>
-      </c>
-      <c r="F58" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B59" t="s">
+      <c r="D59" t="s">
+        <v>9</v>
+      </c>
+      <c r="E59" t="s">
+        <v>10</v>
+      </c>
+      <c r="F59" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
         <v>77</v>
       </c>
-      <c r="D59" t="s">
-        <v>9</v>
-      </c>
-      <c r="E59" t="s">
-        <v>10</v>
-      </c>
-      <c r="F59" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B60" t="s">
+      <c r="D60" t="s">
+        <v>9</v>
+      </c>
+      <c r="E60" t="s">
+        <v>10</v>
+      </c>
+      <c r="F60" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
         <v>78</v>
       </c>
-      <c r="D60" t="s">
-        <v>9</v>
-      </c>
-      <c r="E60" t="s">
-        <v>10</v>
-      </c>
-      <c r="F60" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B61" t="s">
+      <c r="D61" t="s">
+        <v>9</v>
+      </c>
+      <c r="E61" t="s">
+        <v>10</v>
+      </c>
+      <c r="F61" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
         <v>79</v>
       </c>
-      <c r="D61" t="s">
-        <v>18</v>
-      </c>
-      <c r="E61" t="s">
-        <v>10</v>
-      </c>
-      <c r="F61" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B62" t="s">
+      <c r="D62" t="s">
+        <v>18</v>
+      </c>
+      <c r="E62" t="s">
+        <v>10</v>
+      </c>
+      <c r="F62" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
         <v>80</v>
       </c>
-      <c r="D62" t="s">
-        <v>9</v>
-      </c>
-      <c r="E62" t="s">
-        <v>10</v>
-      </c>
-      <c r="F62" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B63" t="s">
+      <c r="D63" t="s">
+        <v>9</v>
+      </c>
+      <c r="E63" t="s">
+        <v>10</v>
+      </c>
+      <c r="F63" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
         <v>81</v>
       </c>
-      <c r="D63" t="s">
-        <v>18</v>
-      </c>
-      <c r="E63" t="s">
-        <v>10</v>
-      </c>
-      <c r="F63" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B64" t="s">
+      <c r="D64" t="s">
+        <v>18</v>
+      </c>
+      <c r="E64" t="s">
+        <v>10</v>
+      </c>
+      <c r="F64" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
         <v>82</v>
       </c>
-      <c r="D64" t="s">
-        <v>18</v>
-      </c>
-      <c r="E64" t="s">
-        <v>10</v>
-      </c>
-      <c r="F64" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B65" t="s">
+      <c r="D65" t="s">
+        <v>18</v>
+      </c>
+      <c r="E65" t="s">
+        <v>10</v>
+      </c>
+      <c r="F65" t="s">
+        <v>15</v>
+      </c>
+      <c r="G65" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
         <v>83</v>
       </c>
-      <c r="D65" t="s">
-        <v>9</v>
-      </c>
-      <c r="E65" t="s">
-        <v>10</v>
-      </c>
-      <c r="F65" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B66" t="s">
+      <c r="D66" t="s">
+        <v>9</v>
+      </c>
+      <c r="E66" t="s">
+        <v>10</v>
+      </c>
+      <c r="F66" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
         <v>84</v>
       </c>
-      <c r="D66" t="s">
-        <v>9</v>
-      </c>
-      <c r="E66" t="s">
-        <v>10</v>
-      </c>
-      <c r="F66" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B67" t="s">
+      <c r="D67" t="s">
+        <v>9</v>
+      </c>
+      <c r="E67" t="s">
+        <v>10</v>
+      </c>
+      <c r="F67" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
         <v>85</v>
       </c>
-      <c r="D67" t="s">
-        <v>9</v>
-      </c>
-      <c r="E67" t="s">
-        <v>10</v>
-      </c>
-      <c r="F67" t="s">
+      <c r="D68" t="s">
+        <v>9</v>
+      </c>
+      <c r="E68" t="s">
+        <v>10</v>
+      </c>
+      <c r="F68" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
+        <v>86</v>
+      </c>
+      <c r="D69" t="s">
+        <v>18</v>
+      </c>
+      <c r="E69" t="s">
+        <v>10</v>
+      </c>
+      <c r="F69" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>87</v>
+      </c>
+      <c r="D70" t="s">
+        <v>18</v>
+      </c>
+      <c r="E70" t="s">
+        <v>10</v>
+      </c>
+      <c r="F70" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
+        <v>88</v>
+      </c>
+      <c r="D71" t="s">
+        <v>18</v>
+      </c>
+      <c r="E71" t="s">
+        <v>10</v>
+      </c>
+      <c r="F71" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="72" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>89</v>
+      </c>
+      <c r="D72" t="s">
+        <v>18</v>
+      </c>
+      <c r="E72" t="s">
+        <v>10</v>
+      </c>
+      <c r="F72" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="73" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
+        <v>90</v>
+      </c>
+      <c r="D73" t="s">
+        <v>18</v>
+      </c>
+      <c r="E73" t="s">
+        <v>10</v>
+      </c>
+      <c r="F73" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="74" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
+        <v>91</v>
+      </c>
+      <c r="D74" t="s">
+        <v>18</v>
+      </c>
+      <c r="E74" t="s">
+        <v>19</v>
+      </c>
+      <c r="F74" t="s">
+        <v>21</v>
+      </c>
+      <c r="G74" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="75" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
+        <v>92</v>
+      </c>
+      <c r="D75" t="s">
+        <v>9</v>
+      </c>
+      <c r="E75" t="s">
+        <v>19</v>
+      </c>
+      <c r="F75" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="76" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
+        <v>93</v>
+      </c>
+      <c r="D76" t="s">
+        <v>9</v>
+      </c>
+      <c r="E76" t="s">
+        <v>19</v>
+      </c>
+      <c r="F76" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="77" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
+        <v>94</v>
+      </c>
+      <c r="D77" t="s">
+        <v>9</v>
+      </c>
+      <c r="E77" t="s">
+        <v>19</v>
+      </c>
+      <c r="F77" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="78" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B78" t="s">
+        <v>95</v>
+      </c>
+      <c r="D78" t="s">
+        <v>18</v>
+      </c>
+      <c r="E78" t="s">
+        <v>19</v>
+      </c>
+      <c r="F78" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="79" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B79" t="s">
+        <v>96</v>
+      </c>
+      <c r="D79" t="s">
+        <v>18</v>
+      </c>
+      <c r="E79" t="s">
+        <v>19</v>
+      </c>
+      <c r="F79" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="80" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B80" t="s">
+        <v>97</v>
+      </c>
+      <c r="D80" t="s">
+        <v>18</v>
+      </c>
+      <c r="E80" t="s">
+        <v>19</v>
+      </c>
+      <c r="F80" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="81" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
+        <v>98</v>
+      </c>
+      <c r="D81" t="s">
+        <v>9</v>
+      </c>
+      <c r="E81" t="s">
+        <v>19</v>
+      </c>
+      <c r="F81" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="82" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
+        <v>99</v>
+      </c>
+      <c r="D82" t="s">
+        <v>9</v>
+      </c>
+      <c r="E82" t="s">
+        <v>19</v>
+      </c>
+      <c r="F82" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>